<commit_message>
added activities to stundenaufzeichnung
</commit_message>
<xml_diff>
--- a/Documents/Sundenauzeichnung.xlsx
+++ b/Documents/Sundenauzeichnung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68157115d40ac8e2/Desktop/School/SYP/Pv-Visualizer/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{75D54FEB-11D0-4CDE-8DE5-18A7CD685A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FB516FD-45B7-4F3E-897A-D4AFF7D8CD09}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3C5BA88-17DC-4378-B87A-8A04948D87DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="16470" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="16470" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,8 +39,36 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Gesamt Stundenanzahl von Sprint 1</t>
+  </si>
   <si>
     <t>Gesamt Stundenanzahl pro Person</t>
   </si>
@@ -54,12 +82,21 @@
     <t>Gesamte Stunden</t>
   </si>
   <si>
+    <t>Lau William</t>
+  </si>
+  <si>
     <t>Erfassungszeitraum</t>
   </si>
   <si>
+    <t>10.10.2022 bis 14.11.2022</t>
+  </si>
+  <si>
     <t>Projektbezeichnung</t>
   </si>
   <si>
+    <t>Pv-Visualizer</t>
+  </si>
+  <si>
     <t>Datum</t>
   </si>
   <si>
@@ -78,70 +115,76 @@
     <t>Stunden</t>
   </si>
   <si>
+    <t>10.10.2022</t>
+  </si>
+  <si>
+    <t>Datenblätter hinzufügen und Clickdummy desgin</t>
+  </si>
+  <si>
+    <t>Create database with an entity and inform fake rest api (Intellij live share)</t>
+  </si>
+  <si>
+    <t>18.10.2022</t>
+  </si>
+  <si>
+    <t>Datenbank mit einer Entity hinzufügen &amp; über Json Fake Api Informieren</t>
+  </si>
+  <si>
+    <t>Grafana installieren, tutorials/dokus lesen</t>
+  </si>
+  <si>
+    <t>Test Json file auf Fake Api laufen lassen</t>
+  </si>
+  <si>
+    <t>Tes Grafana diagramm auf einer embedden(diagramm inahlt wird nicht angezeigt)</t>
+  </si>
+  <si>
+    <t>19.10.2022</t>
+  </si>
+  <si>
+    <t>Daten von Api bekommen / Datenbank &amp; Quarkus Fehler aufgetaucht</t>
+  </si>
+  <si>
+    <t>Fehler in Quarkus beseitigt (Intellij live share)</t>
+  </si>
+  <si>
+    <t>20.10.2022</t>
+  </si>
+  <si>
+    <t>Quarkus Fehler behoben / Entities per Id hinzufügen Fehler und Json file  incorrect</t>
+  </si>
+  <si>
+    <t>github issues anlegen, repos aufräumen, stundenaufzeichnung layout ändern</t>
+  </si>
+  <si>
+    <t>06.11.2022</t>
+  </si>
+  <si>
+    <t>Alle Fehler wegbekommen &amp; neues Json File &amp; Controller</t>
+  </si>
+  <si>
+    <t>Hugo website layouts erstellen(md content pages wollen html layout nicht übernehmen)</t>
+  </si>
+  <si>
+    <t>Grafana hinzufügen / state Fronius implementiert</t>
+  </si>
+  <si>
+    <t>Einfügen des contents der website vorerst auf html page, styles des content, slideshow einfügen</t>
+  </si>
+  <si>
+    <t>Erfolgreich Enities miteinander verknüpft &amp; Grafana Docker File</t>
+  </si>
+  <si>
+    <t>JPA Entites verknüpfen / grafana docker container (intellij live share)</t>
+  </si>
+  <si>
+    <t>14.11.2022</t>
+  </si>
+  <si>
+    <t>Hugo Website Fehler behoben</t>
+  </si>
+  <si>
     <t>Gesamt-Zeit:</t>
-  </si>
-  <si>
-    <t>Sprint 1</t>
-  </si>
-  <si>
-    <t>Lau William</t>
-  </si>
-  <si>
-    <t>Pv-Visualizer</t>
-  </si>
-  <si>
-    <t>Gesamt Stundenanzahl von Sprint 1</t>
-  </si>
-  <si>
-    <t>10.10.2022</t>
-  </si>
-  <si>
-    <t>Datenblätter hinzufügen und Clickdummy desgin</t>
-  </si>
-  <si>
-    <t>18.10.2022</t>
-  </si>
-  <si>
-    <t>Datenbank mit einer Entity hinzufügen &amp; über Json Fake Api Informieren</t>
-  </si>
-  <si>
-    <t>Test Json file auf Fake Api laufen lassen</t>
-  </si>
-  <si>
-    <t>19.10.2022</t>
-  </si>
-  <si>
-    <t>Daten von Api bekommen / Datenbank &amp; Quarkus Fehler aufgetaucht</t>
-  </si>
-  <si>
-    <t>20.10.2022</t>
-  </si>
-  <si>
-    <t>Quarkus Fehler behoben / Entities per Id hinzufügen Fehler und Json file  incorrect</t>
-  </si>
-  <si>
-    <t>06.11.2022</t>
-  </si>
-  <si>
-    <t>Alle Fehler wegbekommen &amp; neues Json File &amp; Controller</t>
-  </si>
-  <si>
-    <t>Grafana hinzufügen / state Fronius implementiert</t>
-  </si>
-  <si>
-    <t>09.11.2022</t>
-  </si>
-  <si>
-    <t>Erfolgreich Enities miteinander verknüpft &amp; Grafana Docker File</t>
-  </si>
-  <si>
-    <t>14.11.2022</t>
-  </si>
-  <si>
-    <t>Hugo Website Fehler behoben</t>
-  </si>
-  <si>
-    <t>10.10.2022 bis 14.11.2022</t>
   </si>
 </sst>
 </file>
@@ -151,7 +194,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[hh]:mm;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +249,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1020,7 +1077,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1146,6 +1203,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="63" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="64" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="65" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="58" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1200,6 +1266,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1257,6 +1332,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1314,30 +1392,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="63" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="64" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="65" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="3" builtinId="24"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="1" builtinId="21"/>
+    <cellStyle name="Ausgabe" xfId="1" builtinId="21"/>
+    <cellStyle name="Berechnung" xfId="2" builtinId="22"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="3" builtinId="24"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1353,7 +1422,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Übersicht"/>
@@ -1367,8 +1436,62 @@
 </externalLink>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>10</v>
+    <v>2</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1637,14 +1760,14 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:I6"/>
+      <selection activeCell="A4" sqref="A4:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="41" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="41"/>
@@ -1655,7 +1778,7 @@
       <c r="H1" s="41"/>
       <c r="I1" s="41"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
       <c r="A2" s="42"/>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
@@ -1666,9 +1789,9 @@
       <c r="H2" s="42"/>
       <c r="I2" s="42"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="A3" s="43" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
@@ -1679,21 +1802,21 @@
       <c r="H3" s="44"/>
       <c r="I3" s="45"/>
     </row>
-    <row r="4" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="105">
+    <row r="4" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A4" s="49" t="e" vm="1">
         <f>[1]Projektstundennachweis!I51+[1]Projektstundennachweis!R51</f>
-        <v>0</v>
-      </c>
-      <c r="B4" s="106"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="107"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1704,9 +1827,9 @@
       <c r="H5" s="4"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1">
       <c r="A6" s="43" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B6" s="44"/>
       <c r="C6" s="44"/>
@@ -1717,7 +1840,7 @@
       <c r="H6" s="44"/>
       <c r="I6" s="45"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.75" thickTop="1">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="7"/>
@@ -1728,14 +1851,14 @@
       <c r="H7" s="1"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="23" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="25"/>
       <c r="D8" s="46" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E8" s="47"/>
       <c r="F8" s="47"/>
@@ -1743,9 +1866,9 @@
       <c r="H8" s="47"/>
       <c r="I8" s="48"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="26" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B9" s="27"/>
       <c r="C9" s="28"/>
@@ -1759,7 +1882,7 @@
       <c r="H9" s="36"/>
       <c r="I9" s="37"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15.75" thickBot="1">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
@@ -1770,14 +1893,14 @@
       <c r="H10" s="9"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="23" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="25"/>
       <c r="D11" s="32" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E11" s="33"/>
       <c r="F11" s="33"/>
@@ -1785,15 +1908,15 @@
       <c r="H11" s="33"/>
       <c r="I11" s="34"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" s="29" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="31"/>
       <c r="D12" s="38">
-        <f>'Sprint 1'!R50</f>
-        <v>0</v>
+        <f>'Sprint 1'!R51</f>
+        <v>0.6680555555555554</v>
       </c>
       <c r="E12" s="39"/>
       <c r="F12" s="39"/>
@@ -1825,248 +1948,248 @@
   <dimension ref="A1:R51"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:F14"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+    <row r="1" spans="1:18" ht="15.75" thickTop="1">
+      <c r="A1" s="104" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="105"/>
+      <c r="C1" s="112" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="104" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="105"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="94"/>
+      <c r="R1" s="95"/>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="96" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="97"/>
+      <c r="C2" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="96" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="97"/>
+      <c r="L2" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="98"/>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="99" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="100"/>
+      <c r="C3" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="108" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="97" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="98"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="88"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="65" t="s">
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="99" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="100"/>
+      <c r="L3" s="101" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
+      <c r="O3" s="101"/>
+      <c r="P3" s="101"/>
+      <c r="Q3" s="101"/>
+      <c r="R3" s="102"/>
+    </row>
+    <row r="4" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A4" s="60"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="61"/>
+      <c r="R4" s="103"/>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A5" s="106" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="107"/>
+      <c r="C5" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="44"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="106" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="107"/>
+      <c r="L5" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="82"/>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" thickTop="1">
+      <c r="A6" s="108"/>
+      <c r="B6" s="109"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="83" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="90"/>
-      <c r="L2" s="65" t="s">
+      <c r="I6" s="85" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="108"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="83" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q6" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="91"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="94" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="93"/>
-      <c r="L3" s="94" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" s="94"/>
-      <c r="N3" s="94"/>
-      <c r="O3" s="94"/>
-      <c r="P3" s="94"/>
-      <c r="Q3" s="94"/>
-      <c r="R3" s="95"/>
-    </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="57"/>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="58"/>
-      <c r="P4" s="58"/>
-      <c r="Q4" s="58"/>
-      <c r="R4" s="96"/>
-    </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="99" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="100"/>
-      <c r="C5" s="67" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="44"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="99" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="100"/>
-      <c r="L5" s="67" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="76"/>
-    </row>
-    <row r="6" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="101"/>
-      <c r="B6" s="102"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="77" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="79" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="101"/>
-      <c r="K6" s="102"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="71"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="72"/>
-      <c r="P6" s="77" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q6" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="R6" s="79" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="101"/>
-      <c r="B7" s="102"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="79"/>
-      <c r="J7" s="101"/>
-      <c r="K7" s="102"/>
-      <c r="L7" s="70"/>
-      <c r="M7" s="71"/>
-      <c r="N7" s="71"/>
-      <c r="O7" s="72"/>
-      <c r="P7" s="77"/>
-      <c r="Q7" s="77"/>
-      <c r="R7" s="79"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="101"/>
-      <c r="B8" s="102"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="79"/>
-      <c r="J8" s="101"/>
-      <c r="K8" s="102"/>
-      <c r="L8" s="70"/>
-      <c r="M8" s="71"/>
-      <c r="N8" s="71"/>
-      <c r="O8" s="72"/>
-      <c r="P8" s="77"/>
-      <c r="Q8" s="77"/>
-      <c r="R8" s="79"/>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="103"/>
-      <c r="B9" s="104"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="103"/>
-      <c r="K9" s="104"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="74"/>
-      <c r="N9" s="74"/>
-      <c r="O9" s="75"/>
-      <c r="P9" s="78"/>
-      <c r="Q9" s="78"/>
-      <c r="R9" s="80"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="81" t="s">
+      <c r="R6" s="85" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="108"/>
+      <c r="B7" s="109"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="109"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="77"/>
+      <c r="O7" s="78"/>
+      <c r="P7" s="83"/>
+      <c r="Q7" s="83"/>
+      <c r="R7" s="85"/>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="108"/>
+      <c r="B8" s="109"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="108"/>
+      <c r="K8" s="109"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="78"/>
+      <c r="P8" s="83"/>
+      <c r="Q8" s="83"/>
+      <c r="R8" s="85"/>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A9" s="110"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="110"/>
+      <c r="K9" s="111"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="81"/>
+      <c r="P9" s="84"/>
+      <c r="Q9" s="84"/>
+      <c r="R9" s="86"/>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="83" t="s">
+      <c r="B10" s="88"/>
+      <c r="C10" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="85"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="91"/>
       <c r="G10" s="11">
         <v>0.5</v>
       </c>
@@ -2077,30 +2200,38 @@
         <f>H10-G10</f>
         <v>6.597222222222221E-2</v>
       </c>
-      <c r="J10" s="81"/>
-      <c r="K10" s="82"/>
-      <c r="L10" s="83"/>
-      <c r="M10" s="84"/>
-      <c r="N10" s="84"/>
-      <c r="O10" s="85"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="12"/>
+      <c r="J10" s="87">
+        <v>44852</v>
+      </c>
+      <c r="K10" s="88"/>
+      <c r="L10" s="89" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="90"/>
+      <c r="N10" s="90"/>
+      <c r="O10" s="91"/>
+      <c r="P10" s="11">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="Q10" s="12">
+        <v>0.64374999999999993</v>
+      </c>
       <c r="R10" s="13">
         <f>Q10-P10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="64" t="s">
+        <v>0.11944444444444435</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="66"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="67" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="69"/>
       <c r="G11" s="14">
         <v>0.53125</v>
       </c>
@@ -2111,30 +2242,38 @@
         <f>H11-G11</f>
         <v>0.11111111111111105</v>
       </c>
-      <c r="J11" s="63"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="65"/>
-      <c r="O11" s="66"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="15"/>
+      <c r="J11" s="66">
+        <v>44853</v>
+      </c>
+      <c r="K11" s="57"/>
+      <c r="L11" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="68"/>
+      <c r="N11" s="68"/>
+      <c r="O11" s="69"/>
+      <c r="P11" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="Q11" s="15">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="R11" s="13">
         <f>Q11-P11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="64" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="66"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="57"/>
+      <c r="C12" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="69"/>
       <c r="G12" s="14">
         <v>0.60763888888888895</v>
       </c>
@@ -2145,30 +2284,38 @@
         <f t="shared" ref="I12:I49" si="0">H12-G12</f>
         <v>3.4722222222222099E-2</v>
       </c>
-      <c r="J12" s="63"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="64"/>
-      <c r="M12" s="65"/>
-      <c r="N12" s="65"/>
-      <c r="O12" s="66"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="15"/>
+      <c r="J12" s="66">
+        <v>44853</v>
+      </c>
+      <c r="K12" s="57"/>
+      <c r="L12" s="70" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12" s="71"/>
+      <c r="N12" s="71"/>
+      <c r="O12" s="72"/>
+      <c r="P12" s="14">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="Q12" s="15">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="R12" s="13">
-        <f t="shared" ref="R12:R37" si="1">Q12-P12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="54"/>
-      <c r="C13" s="64" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="66"/>
+        <f t="shared" ref="R12:R38" si="1">Q12-P12</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="57"/>
+      <c r="C13" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="69"/>
       <c r="G13" s="14">
         <v>0.33333333333333331</v>
       </c>
@@ -2179,30 +2326,38 @@
         <f t="shared" si="0"/>
         <v>0.11805555555555558</v>
       </c>
-      <c r="J13" s="63"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="64"/>
-      <c r="M13" s="65"/>
-      <c r="N13" s="65"/>
-      <c r="O13" s="66"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="15"/>
+      <c r="J13" s="66">
+        <v>44854</v>
+      </c>
+      <c r="K13" s="57"/>
+      <c r="L13" s="67" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="68"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="69"/>
+      <c r="P13" s="14">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="Q13" s="15">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="R13" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="63" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="66"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="66" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="57"/>
+      <c r="C14" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="69"/>
       <c r="G14" s="14">
         <v>0.36805555555555558</v>
       </c>
@@ -2213,30 +2368,38 @@
         <f t="shared" si="0"/>
         <v>8.3333333333333315E-2</v>
       </c>
-      <c r="J14" s="63"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="64"/>
-      <c r="M14" s="65"/>
-      <c r="N14" s="65"/>
-      <c r="O14" s="66"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="15"/>
+      <c r="J14" s="66">
+        <v>44855</v>
+      </c>
+      <c r="K14" s="92"/>
+      <c r="L14" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="M14" s="57"/>
+      <c r="N14" s="57"/>
+      <c r="O14" s="59"/>
+      <c r="P14" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="Q14" s="15">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="R14" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="63" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="54"/>
-      <c r="C15" s="64" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="66"/>
+        <f>Q14-P14</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="57"/>
+      <c r="C15" s="67" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="69"/>
       <c r="G15" s="14">
         <v>0.77083333333333337</v>
       </c>
@@ -2247,30 +2410,38 @@
         <f t="shared" si="0"/>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="J15" s="63"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="65"/>
-      <c r="N15" s="65"/>
-      <c r="O15" s="66"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="15"/>
+      <c r="J15" s="66">
+        <v>44877</v>
+      </c>
+      <c r="K15" s="57"/>
+      <c r="L15" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M15" s="68"/>
+      <c r="N15" s="68"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="Q15" s="15">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="R15" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="63" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="54"/>
-      <c r="C16" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="66"/>
+        <v>0.10416666666666663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="57"/>
+      <c r="C16" s="67" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="69"/>
       <c r="G16" s="14">
         <v>0.85416666666666663</v>
       </c>
@@ -2281,30 +2452,38 @@
         <f t="shared" si="0"/>
         <v>4.1666666666666741E-2</v>
       </c>
-      <c r="J16" s="63"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="64"/>
-      <c r="M16" s="65"/>
-      <c r="N16" s="65"/>
-      <c r="O16" s="66"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="15"/>
+      <c r="J16" s="66">
+        <v>44846</v>
+      </c>
+      <c r="K16" s="57"/>
+      <c r="L16" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="M16" s="68"/>
+      <c r="N16" s="68"/>
+      <c r="O16" s="69"/>
+      <c r="P16" s="14">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="Q16" s="15">
+        <v>0.90277777777777779</v>
+      </c>
       <c r="R16" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="63" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="66"/>
+        <v>9.7222222222222321E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="66">
+        <v>44878</v>
+      </c>
+      <c r="B17" s="57"/>
+      <c r="C17" s="67" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="69"/>
       <c r="G17" s="14">
         <v>0.33333333333333331</v>
       </c>
@@ -2315,30 +2494,38 @@
         <f t="shared" si="0"/>
         <v>0.15625</v>
       </c>
-      <c r="J17" s="63"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="64"/>
-      <c r="M17" s="65"/>
-      <c r="N17" s="65"/>
-      <c r="O17" s="66"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="15"/>
+      <c r="J17" s="66">
+        <v>44878</v>
+      </c>
+      <c r="K17" s="57"/>
+      <c r="L17" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="M17" s="68"/>
+      <c r="N17" s="68"/>
+      <c r="O17" s="69"/>
+      <c r="P17" s="14">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="Q17" s="15">
+        <v>0.49305555555555558</v>
+      </c>
       <c r="R17" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="64" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="66"/>
+        <f>Q17-P17</f>
+        <v>0.1388888888888889</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="66" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="57"/>
+      <c r="C18" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="69"/>
       <c r="G18" s="14">
         <v>0.41666666666666669</v>
       </c>
@@ -2349,12 +2536,12 @@
         <f t="shared" si="0"/>
         <v>8.3333333333333315E-2</v>
       </c>
-      <c r="J18" s="63"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="64"/>
-      <c r="M18" s="65"/>
-      <c r="N18" s="65"/>
-      <c r="O18" s="66"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="67"/>
+      <c r="M18" s="68"/>
+      <c r="N18" s="68"/>
+      <c r="O18" s="69"/>
       <c r="P18" s="14"/>
       <c r="Q18" s="15"/>
       <c r="R18" s="13">
@@ -2362,25 +2549,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="63"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="66"/>
+    <row r="19" spans="1:18">
+      <c r="A19" s="66"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="69"/>
       <c r="G19" s="14"/>
       <c r="H19" s="15"/>
       <c r="I19" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J19" s="63"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="64"/>
-      <c r="M19" s="65"/>
-      <c r="N19" s="65"/>
-      <c r="O19" s="66"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="67"/>
+      <c r="M19" s="68"/>
+      <c r="N19" s="68"/>
+      <c r="O19" s="69"/>
       <c r="P19" s="14"/>
       <c r="Q19" s="15"/>
       <c r="R19" s="13">
@@ -2388,25 +2575,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="63"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="66"/>
+    <row r="20" spans="1:18">
+      <c r="A20" s="66"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="69"/>
       <c r="G20" s="14"/>
       <c r="H20" s="15"/>
       <c r="I20" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J20" s="63"/>
-      <c r="K20" s="54"/>
-      <c r="L20" s="64"/>
-      <c r="M20" s="65"/>
-      <c r="N20" s="65"/>
-      <c r="O20" s="66"/>
+      <c r="J20" s="66"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="67"/>
+      <c r="M20" s="68"/>
+      <c r="N20" s="68"/>
+      <c r="O20" s="69"/>
       <c r="P20" s="14"/>
       <c r="Q20" s="15"/>
       <c r="R20" s="13">
@@ -2414,25 +2601,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="63"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="66"/>
+    <row r="21" spans="1:18">
+      <c r="A21" s="66"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="69"/>
       <c r="G21" s="14"/>
       <c r="H21" s="15"/>
       <c r="I21" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J21" s="63"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="64"/>
-      <c r="M21" s="65"/>
-      <c r="N21" s="65"/>
-      <c r="O21" s="66"/>
+      <c r="J21" s="66"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="67"/>
+      <c r="M21" s="68"/>
+      <c r="N21" s="68"/>
+      <c r="O21" s="69"/>
       <c r="P21" s="14"/>
       <c r="Q21" s="15"/>
       <c r="R21" s="13">
@@ -2440,25 +2627,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="63"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="66"/>
+    <row r="22" spans="1:18">
+      <c r="A22" s="66"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="69"/>
       <c r="G22" s="14"/>
       <c r="H22" s="15"/>
       <c r="I22" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J22" s="63"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="64"/>
-      <c r="M22" s="65"/>
-      <c r="N22" s="65"/>
-      <c r="O22" s="66"/>
+      <c r="J22" s="66"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="67"/>
+      <c r="M22" s="68"/>
+      <c r="N22" s="68"/>
+      <c r="O22" s="69"/>
       <c r="P22" s="14"/>
       <c r="Q22" s="15"/>
       <c r="R22" s="13">
@@ -2466,25 +2653,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="63"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="66"/>
+    <row r="23" spans="1:18">
+      <c r="A23" s="66"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="69"/>
       <c r="G23" s="14"/>
       <c r="H23" s="15"/>
       <c r="I23" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J23" s="63"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="64"/>
-      <c r="M23" s="65"/>
-      <c r="N23" s="65"/>
-      <c r="O23" s="66"/>
+      <c r="J23" s="66"/>
+      <c r="K23" s="57"/>
+      <c r="L23" s="67"/>
+      <c r="M23" s="68"/>
+      <c r="N23" s="68"/>
+      <c r="O23" s="69"/>
       <c r="P23" s="14"/>
       <c r="Q23" s="15"/>
       <c r="R23" s="13">
@@ -2492,51 +2679,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
-      <c r="B24" s="54"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="56"/>
+    <row r="24" spans="1:18">
+      <c r="A24" s="56"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="59"/>
       <c r="G24" s="16"/>
       <c r="H24" s="17"/>
       <c r="I24" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J24" s="53"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="55"/>
-      <c r="M24" s="54"/>
-      <c r="N24" s="54"/>
-      <c r="O24" s="56"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="17"/>
+      <c r="J24" s="66"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="67"/>
+      <c r="M24" s="68"/>
+      <c r="N24" s="68"/>
+      <c r="O24" s="69"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="15"/>
       <c r="R24" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="53"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="56"/>
+    <row r="25" spans="1:18">
+      <c r="A25" s="56"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="59"/>
       <c r="G25" s="16"/>
       <c r="H25" s="17"/>
       <c r="I25" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J25" s="53"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="55"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="54"/>
-      <c r="O25" s="56"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="57"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="57"/>
+      <c r="O25" s="59"/>
       <c r="P25" s="16"/>
       <c r="Q25" s="17"/>
       <c r="R25" s="13">
@@ -2544,25 +2731,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="53"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="56"/>
+    <row r="26" spans="1:18">
+      <c r="A26" s="56"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="59"/>
       <c r="G26" s="16"/>
       <c r="H26" s="17"/>
       <c r="I26" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J26" s="53"/>
-      <c r="K26" s="54"/>
-      <c r="L26" s="55"/>
-      <c r="M26" s="54"/>
-      <c r="N26" s="54"/>
-      <c r="O26" s="56"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="57"/>
+      <c r="N26" s="57"/>
+      <c r="O26" s="59"/>
       <c r="P26" s="16"/>
       <c r="Q26" s="17"/>
       <c r="R26" s="13">
@@ -2570,25 +2757,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="53"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="56"/>
+    <row r="27" spans="1:18">
+      <c r="A27" s="56"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="59"/>
       <c r="G27" s="16"/>
       <c r="H27" s="17"/>
       <c r="I27" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J27" s="53"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="55"/>
-      <c r="M27" s="54"/>
-      <c r="N27" s="54"/>
-      <c r="O27" s="56"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="57"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="57"/>
+      <c r="N27" s="57"/>
+      <c r="O27" s="59"/>
       <c r="P27" s="16"/>
       <c r="Q27" s="17"/>
       <c r="R27" s="13">
@@ -2596,25 +2783,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="53"/>
-      <c r="B28" s="54"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="56"/>
+    <row r="28" spans="1:18">
+      <c r="A28" s="56"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="59"/>
       <c r="G28" s="16"/>
       <c r="H28" s="17"/>
       <c r="I28" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J28" s="53"/>
-      <c r="K28" s="54"/>
-      <c r="L28" s="55"/>
-      <c r="M28" s="54"/>
-      <c r="N28" s="54"/>
-      <c r="O28" s="56"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="57"/>
+      <c r="L28" s="58"/>
+      <c r="M28" s="57"/>
+      <c r="N28" s="57"/>
+      <c r="O28" s="59"/>
       <c r="P28" s="16"/>
       <c r="Q28" s="17"/>
       <c r="R28" s="13">
@@ -2622,25 +2809,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
-      <c r="B29" s="54"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="56"/>
+    <row r="29" spans="1:18">
+      <c r="A29" s="56"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="59"/>
       <c r="G29" s="16"/>
       <c r="H29" s="17"/>
       <c r="I29" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J29" s="53"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="55"/>
-      <c r="M29" s="54"/>
-      <c r="N29" s="54"/>
-      <c r="O29" s="56"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="57"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="57"/>
+      <c r="N29" s="57"/>
+      <c r="O29" s="59"/>
       <c r="P29" s="16"/>
       <c r="Q29" s="17"/>
       <c r="R29" s="13">
@@ -2648,25 +2835,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
-      <c r="B30" s="54"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="56"/>
+    <row r="30" spans="1:18">
+      <c r="A30" s="56"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="59"/>
       <c r="G30" s="16"/>
       <c r="H30" s="17"/>
       <c r="I30" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J30" s="53"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="55"/>
-      <c r="M30" s="54"/>
-      <c r="N30" s="54"/>
-      <c r="O30" s="56"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="58"/>
+      <c r="M30" s="57"/>
+      <c r="N30" s="57"/>
+      <c r="O30" s="59"/>
       <c r="P30" s="16"/>
       <c r="Q30" s="17"/>
       <c r="R30" s="13">
@@ -2674,25 +2861,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
-      <c r="B31" s="54"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="56"/>
+    <row r="31" spans="1:18">
+      <c r="A31" s="56"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="59"/>
       <c r="G31" s="16"/>
       <c r="H31" s="17"/>
       <c r="I31" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J31" s="53"/>
-      <c r="K31" s="54"/>
-      <c r="L31" s="55"/>
-      <c r="M31" s="54"/>
-      <c r="N31" s="54"/>
-      <c r="O31" s="56"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="57"/>
+      <c r="N31" s="57"/>
+      <c r="O31" s="59"/>
       <c r="P31" s="16"/>
       <c r="Q31" s="17"/>
       <c r="R31" s="13">
@@ -2700,25 +2887,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
-      <c r="B32" s="54"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="54"/>
-      <c r="F32" s="56"/>
+    <row r="32" spans="1:18">
+      <c r="A32" s="56"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="59"/>
       <c r="G32" s="16"/>
       <c r="H32" s="17"/>
       <c r="I32" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J32" s="53"/>
-      <c r="K32" s="54"/>
-      <c r="L32" s="55"/>
-      <c r="M32" s="54"/>
-      <c r="N32" s="54"/>
-      <c r="O32" s="56"/>
+      <c r="J32" s="56"/>
+      <c r="K32" s="57"/>
+      <c r="L32" s="58"/>
+      <c r="M32" s="57"/>
+      <c r="N32" s="57"/>
+      <c r="O32" s="59"/>
       <c r="P32" s="16"/>
       <c r="Q32" s="17"/>
       <c r="R32" s="13">
@@ -2726,25 +2913,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="53"/>
-      <c r="B33" s="54"/>
-      <c r="C33" s="55"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="56"/>
+    <row r="33" spans="1:18">
+      <c r="A33" s="56"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="59"/>
       <c r="G33" s="16"/>
       <c r="H33" s="17"/>
       <c r="I33" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J33" s="53"/>
-      <c r="K33" s="54"/>
-      <c r="L33" s="55"/>
-      <c r="M33" s="54"/>
-      <c r="N33" s="54"/>
-      <c r="O33" s="56"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="57"/>
+      <c r="L33" s="58"/>
+      <c r="M33" s="57"/>
+      <c r="N33" s="57"/>
+      <c r="O33" s="59"/>
       <c r="P33" s="16"/>
       <c r="Q33" s="17"/>
       <c r="R33" s="13">
@@ -2752,25 +2939,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="53"/>
-      <c r="B34" s="54"/>
-      <c r="C34" s="55"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="54"/>
-      <c r="F34" s="56"/>
+    <row r="34" spans="1:18">
+      <c r="A34" s="56"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="59"/>
       <c r="G34" s="16"/>
       <c r="H34" s="17"/>
       <c r="I34" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J34" s="53"/>
-      <c r="K34" s="54"/>
-      <c r="L34" s="55"/>
-      <c r="M34" s="54"/>
-      <c r="N34" s="54"/>
-      <c r="O34" s="56"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="57"/>
+      <c r="L34" s="58"/>
+      <c r="M34" s="57"/>
+      <c r="N34" s="57"/>
+      <c r="O34" s="59"/>
       <c r="P34" s="16"/>
       <c r="Q34" s="17"/>
       <c r="R34" s="13">
@@ -2778,25 +2965,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="53"/>
-      <c r="B35" s="54"/>
-      <c r="C35" s="55"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="54"/>
-      <c r="F35" s="56"/>
+    <row r="35" spans="1:18">
+      <c r="A35" s="56"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="59"/>
       <c r="G35" s="16"/>
       <c r="H35" s="17"/>
       <c r="I35" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J35" s="53"/>
-      <c r="K35" s="54"/>
-      <c r="L35" s="55"/>
-      <c r="M35" s="54"/>
-      <c r="N35" s="54"/>
-      <c r="O35" s="56"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="57"/>
+      <c r="L35" s="58"/>
+      <c r="M35" s="57"/>
+      <c r="N35" s="57"/>
+      <c r="O35" s="59"/>
       <c r="P35" s="16"/>
       <c r="Q35" s="17"/>
       <c r="R35" s="13">
@@ -2804,25 +2991,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="53"/>
-      <c r="B36" s="54"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="56"/>
+    <row r="36" spans="1:18">
+      <c r="A36" s="56"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="59"/>
       <c r="G36" s="16"/>
       <c r="H36" s="17"/>
       <c r="I36" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J36" s="53"/>
-      <c r="K36" s="54"/>
-      <c r="L36" s="55"/>
-      <c r="M36" s="54"/>
-      <c r="N36" s="54"/>
-      <c r="O36" s="56"/>
+      <c r="J36" s="56"/>
+      <c r="K36" s="57"/>
+      <c r="L36" s="58"/>
+      <c r="M36" s="57"/>
+      <c r="N36" s="57"/>
+      <c r="O36" s="59"/>
       <c r="P36" s="16"/>
       <c r="Q36" s="17"/>
       <c r="R36" s="13">
@@ -2830,25 +3017,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="53"/>
-      <c r="B37" s="54"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="56"/>
+    <row r="37" spans="1:18">
+      <c r="A37" s="56"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="16"/>
       <c r="H37" s="17"/>
       <c r="I37" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J37" s="53"/>
-      <c r="K37" s="54"/>
-      <c r="L37" s="55"/>
-      <c r="M37" s="54"/>
-      <c r="N37" s="54"/>
-      <c r="O37" s="56"/>
+      <c r="J37" s="56"/>
+      <c r="K37" s="57"/>
+      <c r="L37" s="58"/>
+      <c r="M37" s="57"/>
+      <c r="N37" s="57"/>
+      <c r="O37" s="59"/>
       <c r="P37" s="16"/>
       <c r="Q37" s="17"/>
       <c r="R37" s="13">
@@ -2856,103 +3043,103 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="61"/>
-      <c r="B38" s="62"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="54"/>
-      <c r="F38" s="56"/>
+    <row r="38" spans="1:18">
+      <c r="A38" s="64"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="59"/>
       <c r="G38" s="18"/>
       <c r="H38" s="5"/>
       <c r="I38" s="13">
         <f>H38-G38</f>
         <v>0</v>
       </c>
-      <c r="J38" s="61"/>
-      <c r="K38" s="62"/>
-      <c r="L38" s="55"/>
-      <c r="M38" s="54"/>
-      <c r="N38" s="54"/>
-      <c r="O38" s="56"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="5"/>
+      <c r="J38" s="56"/>
+      <c r="K38" s="57"/>
+      <c r="L38" s="58"/>
+      <c r="M38" s="57"/>
+      <c r="N38" s="57"/>
+      <c r="O38" s="59"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="17"/>
       <c r="R38" s="13">
-        <f>Q38-P38</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="53"/>
-      <c r="B39" s="54"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="54"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="56"/>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39" s="56"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="59"/>
       <c r="G39" s="16"/>
       <c r="H39" s="17"/>
       <c r="I39" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J39" s="53"/>
-      <c r="K39" s="54"/>
-      <c r="L39" s="55"/>
-      <c r="M39" s="54"/>
-      <c r="N39" s="54"/>
-      <c r="O39" s="56"/>
-      <c r="P39" s="16"/>
-      <c r="Q39" s="17"/>
+      <c r="J39" s="64"/>
+      <c r="K39" s="65"/>
+      <c r="L39" s="58"/>
+      <c r="M39" s="57"/>
+      <c r="N39" s="57"/>
+      <c r="O39" s="59"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="5"/>
       <c r="R39" s="13">
-        <f t="shared" ref="R39:R49" si="2">Q39-P39</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="53"/>
-      <c r="B40" s="54"/>
-      <c r="C40" s="55"/>
-      <c r="D40" s="54"/>
-      <c r="E40" s="54"/>
-      <c r="F40" s="56"/>
+        <f>Q39-P39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40" s="56"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="59"/>
       <c r="G40" s="16"/>
       <c r="H40" s="17"/>
       <c r="I40" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J40" s="53"/>
-      <c r="K40" s="54"/>
-      <c r="L40" s="55"/>
-      <c r="M40" s="54"/>
-      <c r="N40" s="54"/>
-      <c r="O40" s="56"/>
+      <c r="J40" s="56"/>
+      <c r="K40" s="57"/>
+      <c r="L40" s="58"/>
+      <c r="M40" s="57"/>
+      <c r="N40" s="57"/>
+      <c r="O40" s="59"/>
       <c r="P40" s="16"/>
       <c r="Q40" s="17"/>
       <c r="R40" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="53"/>
-      <c r="B41" s="54"/>
-      <c r="C41" s="55"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="54"/>
-      <c r="F41" s="56"/>
+        <f t="shared" ref="R40:R50" si="2">Q40-P40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41" s="56"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="59"/>
       <c r="G41" s="16"/>
       <c r="H41" s="17"/>
       <c r="I41" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J41" s="53"/>
-      <c r="K41" s="54"/>
-      <c r="L41" s="55"/>
-      <c r="M41" s="54"/>
-      <c r="N41" s="54"/>
-      <c r="O41" s="56"/>
+      <c r="J41" s="56"/>
+      <c r="K41" s="57"/>
+      <c r="L41" s="58"/>
+      <c r="M41" s="57"/>
+      <c r="N41" s="57"/>
+      <c r="O41" s="59"/>
       <c r="P41" s="16"/>
       <c r="Q41" s="17"/>
       <c r="R41" s="13">
@@ -2960,25 +3147,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="53"/>
-      <c r="B42" s="54"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54"/>
-      <c r="F42" s="56"/>
+    <row r="42" spans="1:18">
+      <c r="A42" s="56"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="59"/>
       <c r="G42" s="16"/>
       <c r="H42" s="17"/>
       <c r="I42" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J42" s="53"/>
-      <c r="K42" s="54"/>
-      <c r="L42" s="55"/>
-      <c r="M42" s="54"/>
-      <c r="N42" s="54"/>
-      <c r="O42" s="56"/>
+      <c r="J42" s="56"/>
+      <c r="K42" s="57"/>
+      <c r="L42" s="58"/>
+      <c r="M42" s="57"/>
+      <c r="N42" s="57"/>
+      <c r="O42" s="59"/>
       <c r="P42" s="16"/>
       <c r="Q42" s="17"/>
       <c r="R42" s="13">
@@ -2986,25 +3173,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="53"/>
-      <c r="B43" s="54"/>
-      <c r="C43" s="55"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="54"/>
-      <c r="F43" s="56"/>
+    <row r="43" spans="1:18">
+      <c r="A43" s="56"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="59"/>
       <c r="G43" s="16"/>
       <c r="H43" s="17"/>
       <c r="I43" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J43" s="53"/>
-      <c r="K43" s="54"/>
-      <c r="L43" s="55"/>
-      <c r="M43" s="54"/>
-      <c r="N43" s="54"/>
-      <c r="O43" s="56"/>
+      <c r="J43" s="56"/>
+      <c r="K43" s="57"/>
+      <c r="L43" s="58"/>
+      <c r="M43" s="57"/>
+      <c r="N43" s="57"/>
+      <c r="O43" s="59"/>
       <c r="P43" s="16"/>
       <c r="Q43" s="17"/>
       <c r="R43" s="13">
@@ -3012,25 +3199,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="53"/>
-      <c r="B44" s="54"/>
-      <c r="C44" s="55"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="54"/>
-      <c r="F44" s="56"/>
+    <row r="44" spans="1:18">
+      <c r="A44" s="56"/>
+      <c r="B44" s="57"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="59"/>
       <c r="G44" s="16"/>
       <c r="H44" s="17"/>
       <c r="I44" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J44" s="53"/>
-      <c r="K44" s="54"/>
-      <c r="L44" s="55"/>
-      <c r="M44" s="54"/>
-      <c r="N44" s="54"/>
-      <c r="O44" s="56"/>
+      <c r="J44" s="56"/>
+      <c r="K44" s="57"/>
+      <c r="L44" s="58"/>
+      <c r="M44" s="57"/>
+      <c r="N44" s="57"/>
+      <c r="O44" s="59"/>
       <c r="P44" s="16"/>
       <c r="Q44" s="17"/>
       <c r="R44" s="13">
@@ -3038,25 +3225,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="53"/>
-      <c r="B45" s="54"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="54"/>
-      <c r="E45" s="54"/>
-      <c r="F45" s="56"/>
+    <row r="45" spans="1:18">
+      <c r="A45" s="56"/>
+      <c r="B45" s="57"/>
+      <c r="C45" s="58"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="59"/>
       <c r="G45" s="16"/>
       <c r="H45" s="17"/>
       <c r="I45" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J45" s="53"/>
-      <c r="K45" s="54"/>
-      <c r="L45" s="55"/>
-      <c r="M45" s="54"/>
-      <c r="N45" s="54"/>
-      <c r="O45" s="56"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="57"/>
+      <c r="L45" s="58"/>
+      <c r="M45" s="57"/>
+      <c r="N45" s="57"/>
+      <c r="O45" s="59"/>
       <c r="P45" s="16"/>
       <c r="Q45" s="17"/>
       <c r="R45" s="13">
@@ -3064,25 +3251,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="53"/>
-      <c r="B46" s="54"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="54"/>
-      <c r="F46" s="56"/>
+    <row r="46" spans="1:18">
+      <c r="A46" s="56"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="59"/>
       <c r="G46" s="16"/>
       <c r="H46" s="17"/>
       <c r="I46" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J46" s="53"/>
-      <c r="K46" s="54"/>
-      <c r="L46" s="55"/>
-      <c r="M46" s="54"/>
-      <c r="N46" s="54"/>
-      <c r="O46" s="56"/>
+      <c r="J46" s="56"/>
+      <c r="K46" s="57"/>
+      <c r="L46" s="58"/>
+      <c r="M46" s="57"/>
+      <c r="N46" s="57"/>
+      <c r="O46" s="59"/>
       <c r="P46" s="16"/>
       <c r="Q46" s="17"/>
       <c r="R46" s="13">
@@ -3090,25 +3277,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="53"/>
-      <c r="B47" s="54"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="54"/>
-      <c r="E47" s="54"/>
-      <c r="F47" s="56"/>
+    <row r="47" spans="1:18">
+      <c r="A47" s="56"/>
+      <c r="B47" s="57"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="59"/>
       <c r="G47" s="16"/>
       <c r="H47" s="17"/>
       <c r="I47" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J47" s="53"/>
-      <c r="K47" s="54"/>
-      <c r="L47" s="55"/>
-      <c r="M47" s="54"/>
-      <c r="N47" s="54"/>
-      <c r="O47" s="56"/>
+      <c r="J47" s="56"/>
+      <c r="K47" s="57"/>
+      <c r="L47" s="58"/>
+      <c r="M47" s="57"/>
+      <c r="N47" s="57"/>
+      <c r="O47" s="59"/>
       <c r="P47" s="16"/>
       <c r="Q47" s="17"/>
       <c r="R47" s="13">
@@ -3116,25 +3303,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="53"/>
-      <c r="B48" s="54"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="54"/>
-      <c r="E48" s="54"/>
-      <c r="F48" s="56"/>
+    <row r="48" spans="1:18">
+      <c r="A48" s="56"/>
+      <c r="B48" s="57"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="59"/>
       <c r="G48" s="16"/>
       <c r="H48" s="17"/>
       <c r="I48" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J48" s="53"/>
-      <c r="K48" s="54"/>
-      <c r="L48" s="55"/>
-      <c r="M48" s="54"/>
-      <c r="N48" s="54"/>
-      <c r="O48" s="56"/>
+      <c r="J48" s="56"/>
+      <c r="K48" s="57"/>
+      <c r="L48" s="58"/>
+      <c r="M48" s="57"/>
+      <c r="N48" s="57"/>
+      <c r="O48" s="59"/>
       <c r="P48" s="16"/>
       <c r="Q48" s="17"/>
       <c r="R48" s="13">
@@ -3142,65 +3329,78 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="57"/>
-      <c r="B49" s="58"/>
-      <c r="C49" s="59"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="60"/>
+    <row r="49" spans="1:18">
+      <c r="A49" s="60"/>
+      <c r="B49" s="61"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="61"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="63"/>
       <c r="G49" s="19"/>
       <c r="H49" s="20"/>
       <c r="I49" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J49" s="57"/>
-      <c r="K49" s="58"/>
-      <c r="L49" s="59"/>
-      <c r="M49" s="58"/>
-      <c r="N49" s="58"/>
-      <c r="O49" s="60"/>
-      <c r="P49" s="19"/>
-      <c r="Q49" s="20"/>
-      <c r="R49" s="21">
+      <c r="J49" s="56"/>
+      <c r="K49" s="57"/>
+      <c r="L49" s="58"/>
+      <c r="M49" s="57"/>
+      <c r="N49" s="57"/>
+      <c r="O49" s="59"/>
+      <c r="P49" s="16"/>
+      <c r="Q49" s="17"/>
+      <c r="R49" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="49"/>
-      <c r="B50" s="50"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="52"/>
-      <c r="E50" s="52"/>
-      <c r="F50" s="50"/>
-      <c r="G50" s="51" t="s">
-        <v>12</v>
-      </c>
-      <c r="H50" s="50"/>
+    <row r="50" spans="1:18">
+      <c r="A50" s="52"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="55"/>
+      <c r="E50" s="55"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="H50" s="53"/>
       <c r="I50" s="22">
         <f>SUM(I10:I49)</f>
         <v>0.77777777777777746</v>
       </c>
-      <c r="J50" s="49"/>
-      <c r="K50" s="50"/>
-      <c r="L50" s="51"/>
-      <c r="M50" s="52"/>
-      <c r="N50" s="52"/>
-      <c r="O50" s="50"/>
-      <c r="P50" s="51" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q50" s="50"/>
-      <c r="R50" s="22">
-        <f>SUM(R10:R49)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="J50" s="60"/>
+      <c r="K50" s="61"/>
+      <c r="L50" s="62"/>
+      <c r="M50" s="61"/>
+      <c r="N50" s="61"/>
+      <c r="O50" s="63"/>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="20"/>
+      <c r="R50" s="21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18">
+      <c r="J51" s="52"/>
+      <c r="K51" s="53"/>
+      <c r="L51" s="54"/>
+      <c r="M51" s="55"/>
+      <c r="N51" s="55"/>
+      <c r="O51" s="53"/>
+      <c r="P51" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q51" s="53"/>
+      <c r="R51" s="22">
+        <f>SUM(R10:R50)</f>
+        <v>0.6680555555555554</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="192">
+  <mergeCells count="194">
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A5:B9"/>
     <mergeCell ref="C5:F9"/>
@@ -3298,8 +3498,8 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="J5:K9"/>
     <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J20:K20"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="C46:F46"/>
     <mergeCell ref="A47:B47"/>
@@ -3313,8 +3513,8 @@
     <mergeCell ref="L12:O12"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="L13:O13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L15:O15"/>
     <mergeCell ref="L5:O9"/>
     <mergeCell ref="P5:R5"/>
     <mergeCell ref="P6:P9"/>
@@ -3322,77 +3522,79 @@
     <mergeCell ref="R6:R9"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="L10:O10"/>
-    <mergeCell ref="L19:O19"/>
-    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:O14"/>
     <mergeCell ref="L20:O20"/>
     <mergeCell ref="J21:K21"/>
     <mergeCell ref="L21:O21"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="L22:O22"/>
-    <mergeCell ref="L15:O15"/>
-    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:O23"/>
     <mergeCell ref="L16:O16"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="L17:O17"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="L18:O18"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:O19"/>
     <mergeCell ref="J27:K27"/>
     <mergeCell ref="L27:O27"/>
     <mergeCell ref="J28:K28"/>
     <mergeCell ref="L28:O28"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:O29"/>
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="L24:O24"/>
     <mergeCell ref="J25:K25"/>
     <mergeCell ref="L25:O25"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:O32"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:O26"/>
     <mergeCell ref="J33:K33"/>
     <mergeCell ref="L33:O33"/>
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="L34:O34"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:O29"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="L35:O35"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="L30:O30"/>
     <mergeCell ref="J31:K31"/>
     <mergeCell ref="L31:O31"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="L38:O38"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:O32"/>
     <mergeCell ref="J39:K39"/>
     <mergeCell ref="L39:O39"/>
     <mergeCell ref="J40:K40"/>
     <mergeCell ref="L40:O40"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="L35:O35"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L41:O41"/>
     <mergeCell ref="J36:K36"/>
     <mergeCell ref="L36:O36"/>
     <mergeCell ref="J37:K37"/>
     <mergeCell ref="L37:O37"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="L38:O38"/>
     <mergeCell ref="J45:K45"/>
     <mergeCell ref="L45:O45"/>
     <mergeCell ref="J46:K46"/>
     <mergeCell ref="L46:O46"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="L41:O41"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="L47:O47"/>
     <mergeCell ref="J42:K42"/>
     <mergeCell ref="L42:O42"/>
     <mergeCell ref="J43:K43"/>
     <mergeCell ref="L43:O43"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="L50:O50"/>
-    <mergeCell ref="P50:Q50"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="L47:O47"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="L51:O51"/>
+    <mergeCell ref="P51:Q51"/>
     <mergeCell ref="J48:K48"/>
     <mergeCell ref="L48:O48"/>
     <mergeCell ref="J49:K49"/>
     <mergeCell ref="L49:O49"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="L50:O50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>